<commit_message>
:green_book: Add test data
</commit_message>
<xml_diff>
--- a/tests/testthat/excels/miyagi.xlsx
+++ b/tests/testthat/excels/miyagi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahayashi/Documents/GitHub/lucifer/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahayashi/Documents/GitHub/lucifer/tests/testthat/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036D5A4D-ABC5-5648-9109-D197A0515DD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FDC48E-AA39-464F-9A72-8A111E57553F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="57600" windowHeight="31960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -110,13 +108,6 @@
   </si>
   <si>
     <t>マアジ</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>サバ類（マサバ＋ゴマサバ）</t>
-    <rPh sb="2" eb="3">
-      <t>ルイ</t>
-    </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -332,6 +323,9 @@
       <t>ネン</t>
     </rPh>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>サバ類（マサバ＋ゴマサバ）</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1340,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A4:BM159"/>
+  <dimension ref="A1:BM159"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Z90" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="BN148" sqref="BN148"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1403,6 +1397,39 @@
     <col min="64" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:63">
+      <c r="C1" s="1"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:63">
+      <c r="AI2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AQ2" s="16"/>
+      <c r="AS2" s="16"/>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="16"/>
+    </row>
     <row r="4" spans="1:63" ht="17">
       <c r="A4" s="7" t="s">
         <v>21</v>
@@ -1421,7 +1448,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="Q4" s="44" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="R4" s="42"/>
       <c r="S4" s="42"/>
@@ -1437,7 +1464,7 @@
       <c r="AC4" s="42"/>
       <c r="AD4" s="42"/>
       <c r="AG4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AH4" s="9"/>
       <c r="AI4" s="9"/>
@@ -1453,7 +1480,7 @@
       <c r="AS4" s="9"/>
       <c r="AT4" s="9"/>
       <c r="AW4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AX4" s="5"/>
       <c r="AY4" s="5"/>
@@ -1591,7 +1618,7 @@
         <v>15</v>
       </c>
       <c r="O6" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="70" t="s">
         <v>2</v>
@@ -1636,7 +1663,7 @@
         <v>15</v>
       </c>
       <c r="AE6" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG6" s="27" t="s">
         <v>2</v>
@@ -1681,7 +1708,7 @@
         <v>15</v>
       </c>
       <c r="AU6" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AW6" s="27" t="s">
         <v>2</v>
@@ -1726,12 +1753,12 @@
         <v>15</v>
       </c>
       <c r="BK6" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="14">
       <c r="A7" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="86">
         <v>1</v>
@@ -1775,7 +1802,7 @@
       </c>
       <c r="O7" s="97"/>
       <c r="Q7" s="71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R7" s="84">
         <f>B7+1200</f>
@@ -1830,7 +1857,7 @@
       </c>
       <c r="AE7" s="97"/>
       <c r="AG7" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AH7" s="84">
         <f>R7+1200</f>
@@ -1885,7 +1912,7 @@
       </c>
       <c r="AU7" s="97"/>
       <c r="AW7" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AX7" s="84">
         <f>AH7+1200</f>
@@ -1942,7 +1969,7 @@
     </row>
     <row r="8" spans="1:63" ht="14">
       <c r="A8" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="86">
         <v>13</v>
@@ -1989,7 +2016,7 @@
         <v>39</v>
       </c>
       <c r="Q8" s="72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R8" s="84">
         <f t="shared" ref="R8:R31" si="25">B8+1200</f>
@@ -2047,7 +2074,7 @@
         <v>3639</v>
       </c>
       <c r="AG8" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH8" s="84">
         <f t="shared" ref="AH8:AH31" si="38">R8+1200</f>
@@ -2105,7 +2132,7 @@
         <v>7239</v>
       </c>
       <c r="AW8" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX8" s="84">
         <f t="shared" ref="AX8:AX31" si="40">AH8+1200</f>
@@ -2165,7 +2192,7 @@
     </row>
     <row r="9" spans="1:63" ht="14">
       <c r="A9" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="86">
         <v>25</v>
@@ -2212,7 +2239,7 @@
         <v>75</v>
       </c>
       <c r="Q9" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R9" s="84">
         <f t="shared" si="25"/>
@@ -2270,7 +2297,7 @@
         <v>3675</v>
       </c>
       <c r="AG9" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH9" s="84">
         <f t="shared" si="38"/>
@@ -2328,7 +2355,7 @@
         <v>7275</v>
       </c>
       <c r="AW9" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX9" s="84">
         <f t="shared" si="40"/>
@@ -2388,7 +2415,7 @@
     </row>
     <row r="10" spans="1:63" ht="14">
       <c r="A10" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="86">
         <v>37</v>
@@ -2435,7 +2462,7 @@
         <v>111</v>
       </c>
       <c r="Q10" s="72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R10" s="84">
         <f t="shared" si="25"/>
@@ -2493,7 +2520,7 @@
         <v>3711</v>
       </c>
       <c r="AG10" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH10" s="84">
         <f t="shared" si="38"/>
@@ -2551,7 +2578,7 @@
         <v>7311</v>
       </c>
       <c r="AW10" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX10" s="84">
         <f t="shared" si="40"/>
@@ -2611,7 +2638,7 @@
     </row>
     <row r="11" spans="1:63" ht="14">
       <c r="A11" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="86">
         <v>49</v>
@@ -2658,7 +2685,7 @@
         <v>147</v>
       </c>
       <c r="Q11" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R11" s="84">
         <f t="shared" si="25"/>
@@ -2716,7 +2743,7 @@
         <v>3747</v>
       </c>
       <c r="AG11" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH11" s="84">
         <f t="shared" si="38"/>
@@ -2774,7 +2801,7 @@
         <v>7347</v>
       </c>
       <c r="AW11" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX11" s="84">
         <f t="shared" si="40"/>
@@ -2834,7 +2861,7 @@
     </row>
     <row r="12" spans="1:63" ht="14">
       <c r="A12" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="86">
         <v>61</v>
@@ -2881,7 +2908,7 @@
         <v>183</v>
       </c>
       <c r="Q12" s="72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R12" s="84">
         <f t="shared" si="25"/>
@@ -2939,7 +2966,7 @@
         <v>3783</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH12" s="84">
         <f t="shared" si="38"/>
@@ -2997,7 +3024,7 @@
         <v>7383</v>
       </c>
       <c r="AW12" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AX12" s="84">
         <f t="shared" si="40"/>
@@ -3057,7 +3084,7 @@
     </row>
     <row r="13" spans="1:63" ht="14">
       <c r="A13" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="86">
         <v>73</v>
@@ -3104,7 +3131,7 @@
         <v>219</v>
       </c>
       <c r="Q13" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R13" s="84">
         <f t="shared" si="25"/>
@@ -3162,7 +3189,7 @@
         <v>3819</v>
       </c>
       <c r="AG13" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AH13" s="84">
         <f t="shared" si="38"/>
@@ -3221,7 +3248,7 @@
         <v>7419</v>
       </c>
       <c r="AW13" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AX13" s="84">
         <f t="shared" si="40"/>
@@ -3282,7 +3309,7 @@
     </row>
     <row r="14" spans="1:63" ht="14">
       <c r="A14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="86">
         <v>85</v>
@@ -3329,7 +3356,7 @@
         <v>255</v>
       </c>
       <c r="Q14" s="72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R14" s="84">
         <f t="shared" si="25"/>
@@ -3388,7 +3415,7 @@
         <v>3855</v>
       </c>
       <c r="AG14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH14" s="84">
         <f t="shared" si="38"/>
@@ -3447,7 +3474,7 @@
         <v>7455</v>
       </c>
       <c r="AW14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX14" s="84">
         <f t="shared" si="40"/>
@@ -3508,7 +3535,7 @@
     </row>
     <row r="15" spans="1:63" ht="14">
       <c r="A15" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="86">
         <v>97</v>
@@ -3555,7 +3582,7 @@
         <v>291</v>
       </c>
       <c r="Q15" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R15" s="84">
         <f t="shared" si="25"/>
@@ -3614,7 +3641,7 @@
         <v>3891</v>
       </c>
       <c r="AG15" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH15" s="84">
         <f t="shared" si="38"/>
@@ -3673,7 +3700,7 @@
         <v>7491</v>
       </c>
       <c r="AW15" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX15" s="84">
         <f t="shared" si="40"/>
@@ -3734,7 +3761,7 @@
     </row>
     <row r="16" spans="1:63" ht="14">
       <c r="A16" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="86">
         <v>109</v>
@@ -3781,7 +3808,7 @@
         <v>327</v>
       </c>
       <c r="Q16" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R16" s="84">
         <f t="shared" si="25"/>
@@ -3840,7 +3867,7 @@
         <v>3927</v>
       </c>
       <c r="AG16" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH16" s="84">
         <f t="shared" si="38"/>
@@ -3899,7 +3926,7 @@
         <v>7527</v>
       </c>
       <c r="AW16" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AX16" s="84">
         <f t="shared" si="40"/>
@@ -3960,7 +3987,7 @@
     </row>
     <row r="17" spans="1:65" ht="14">
       <c r="A17" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="86">
         <v>121</v>
@@ -4007,7 +4034,7 @@
         <v>363</v>
       </c>
       <c r="Q17" s="71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R17" s="84">
         <f t="shared" si="25"/>
@@ -4065,7 +4092,7 @@
         <v>3963</v>
       </c>
       <c r="AG17" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH17" s="84">
         <f t="shared" si="38"/>
@@ -4123,7 +4150,7 @@
         <v>7563</v>
       </c>
       <c r="AW17" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX17" s="84">
         <f t="shared" si="40"/>
@@ -4183,7 +4210,7 @@
     </row>
     <row r="18" spans="1:65" ht="14">
       <c r="A18" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="86">
         <v>133</v>
@@ -4230,7 +4257,7 @@
         <v>399</v>
       </c>
       <c r="Q18" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R18" s="84">
         <f t="shared" si="25"/>
@@ -4289,7 +4316,7 @@
         <v>3999</v>
       </c>
       <c r="AG18" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH18" s="84">
         <f t="shared" si="38"/>
@@ -4348,7 +4375,7 @@
         <v>7599</v>
       </c>
       <c r="AW18" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX18" s="84">
         <f t="shared" si="40"/>
@@ -4409,7 +4436,7 @@
     </row>
     <row r="19" spans="1:65" ht="14">
       <c r="A19" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="86">
         <v>145</v>
@@ -4456,7 +4483,7 @@
         <v>435</v>
       </c>
       <c r="Q19" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R19" s="84">
         <f t="shared" si="25"/>
@@ -4514,7 +4541,7 @@
         <v>4035</v>
       </c>
       <c r="AG19" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH19" s="84">
         <f t="shared" si="38"/>
@@ -4572,7 +4599,7 @@
         <v>7635</v>
       </c>
       <c r="AW19" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX19" s="84">
         <f t="shared" si="40"/>
@@ -4633,7 +4660,7 @@
     </row>
     <row r="20" spans="1:65" ht="14">
       <c r="A20" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="86">
         <v>157</v>
@@ -4680,7 +4707,7 @@
         <v>471</v>
       </c>
       <c r="Q20" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R20" s="84">
         <f t="shared" si="25"/>
@@ -4739,7 +4766,7 @@
         <v>4071</v>
       </c>
       <c r="AG20" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH20" s="84">
         <f t="shared" si="38"/>
@@ -4798,7 +4825,7 @@
         <v>7671</v>
       </c>
       <c r="AW20" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX20" s="84">
         <f t="shared" si="40"/>
@@ -4859,7 +4886,7 @@
     </row>
     <row r="21" spans="1:65" ht="14">
       <c r="A21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="86">
         <v>169</v>
@@ -4906,7 +4933,7 @@
         <v>507</v>
       </c>
       <c r="Q21" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R21" s="84">
         <f t="shared" si="25"/>
@@ -4965,7 +4992,7 @@
         <v>4107</v>
       </c>
       <c r="AG21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH21" s="84">
         <f t="shared" si="38"/>
@@ -5024,7 +5051,7 @@
         <v>7707</v>
       </c>
       <c r="AW21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX21" s="84">
         <f t="shared" si="40"/>
@@ -5085,7 +5112,7 @@
     </row>
     <row r="22" spans="1:65" ht="14">
       <c r="A22" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="86">
         <v>181</v>
@@ -5133,7 +5160,7 @@
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R22" s="84">
         <f t="shared" si="25"/>
@@ -5193,7 +5220,7 @@
       </c>
       <c r="AF22" s="11"/>
       <c r="AG22" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH22" s="84">
         <f t="shared" si="38"/>
@@ -5253,7 +5280,7 @@
       </c>
       <c r="AV22" s="11"/>
       <c r="AW22" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX22" s="84">
         <f t="shared" si="40"/>
@@ -5316,7 +5343,7 @@
     </row>
     <row r="23" spans="1:65" ht="14">
       <c r="A23" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="86">
         <v>193</v>
@@ -5363,7 +5390,7 @@
         <v>579</v>
       </c>
       <c r="Q23" s="71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R23" s="84">
         <f t="shared" si="25"/>
@@ -5422,7 +5449,7 @@
         <v>4179</v>
       </c>
       <c r="AG23" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH23" s="84">
         <f t="shared" si="38"/>
@@ -5481,7 +5508,7 @@
         <v>7779</v>
       </c>
       <c r="AW23" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX23" s="84">
         <f t="shared" si="40"/>
@@ -5542,7 +5569,7 @@
     </row>
     <row r="24" spans="1:65" ht="14">
       <c r="A24" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="86">
         <v>205</v>
@@ -5589,7 +5616,7 @@
         <v>615</v>
       </c>
       <c r="Q24" s="72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R24" s="84">
         <f t="shared" si="25"/>
@@ -5648,7 +5675,7 @@
         <v>4215</v>
       </c>
       <c r="AG24" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH24" s="84">
         <f t="shared" si="38"/>
@@ -5707,7 +5734,7 @@
         <v>7815</v>
       </c>
       <c r="AW24" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX24" s="84">
         <f t="shared" si="40"/>
@@ -5768,7 +5795,7 @@
     </row>
     <row r="25" spans="1:65" ht="14">
       <c r="A25" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="86">
         <v>217</v>
@@ -5815,7 +5842,7 @@
         <v>651</v>
       </c>
       <c r="Q25" s="71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R25" s="84">
         <f t="shared" si="25"/>
@@ -5874,7 +5901,7 @@
         <v>4251</v>
       </c>
       <c r="AG25" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH25" s="84">
         <f t="shared" si="38"/>
@@ -5933,7 +5960,7 @@
         <v>7851</v>
       </c>
       <c r="AW25" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AX25" s="84">
         <f t="shared" si="40"/>
@@ -5994,7 +6021,7 @@
     </row>
     <row r="26" spans="1:65" ht="14">
       <c r="A26" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="86">
         <v>229</v>
@@ -6041,7 +6068,7 @@
         <v>687</v>
       </c>
       <c r="Q26" s="72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R26" s="84">
         <f t="shared" si="25"/>
@@ -6100,7 +6127,7 @@
         <v>4287</v>
       </c>
       <c r="AG26" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH26" s="84">
         <f t="shared" si="38"/>
@@ -6159,7 +6186,7 @@
         <v>7887</v>
       </c>
       <c r="AW26" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX26" s="84">
         <f t="shared" si="40"/>
@@ -6220,7 +6247,7 @@
     </row>
     <row r="27" spans="1:65" ht="14">
       <c r="A27" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="86">
         <v>241</v>
@@ -6267,7 +6294,7 @@
         <v>723</v>
       </c>
       <c r="Q27" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R27" s="84">
         <f t="shared" si="25"/>
@@ -6326,7 +6353,7 @@
         <v>4323</v>
       </c>
       <c r="AG27" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH27" s="84">
         <f t="shared" si="38"/>
@@ -6385,7 +6412,7 @@
         <v>7923</v>
       </c>
       <c r="AW27" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX27" s="84">
         <f t="shared" si="40"/>
@@ -6446,7 +6473,7 @@
     </row>
     <row r="28" spans="1:65" ht="14">
       <c r="A28" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="86">
         <v>253</v>
@@ -6493,7 +6520,7 @@
         <v>759</v>
       </c>
       <c r="Q28" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R28" s="84">
         <f t="shared" si="25"/>
@@ -6552,7 +6579,7 @@
         <v>4359</v>
       </c>
       <c r="AG28" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH28" s="84">
         <f t="shared" si="38"/>
@@ -6611,7 +6638,7 @@
         <v>7959</v>
       </c>
       <c r="AW28" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AX28" s="84">
         <f t="shared" si="40"/>
@@ -6672,7 +6699,7 @@
     </row>
     <row r="29" spans="1:65" ht="14">
       <c r="A29" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="86">
         <v>265</v>
@@ -6720,7 +6747,7 @@
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R29" s="84">
         <f t="shared" si="25"/>
@@ -6779,7 +6806,7 @@
         <v>4395</v>
       </c>
       <c r="AG29" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH29" s="84">
         <f t="shared" si="38"/>
@@ -6838,7 +6865,7 @@
         <v>7995</v>
       </c>
       <c r="AW29" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX29" s="84">
         <f t="shared" si="40"/>
@@ -6899,7 +6926,7 @@
     </row>
     <row r="30" spans="1:65" ht="14">
       <c r="A30" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="86">
         <v>277</v>
@@ -6947,7 +6974,7 @@
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R30" s="84">
         <f t="shared" si="25"/>
@@ -7007,7 +7034,7 @@
       </c>
       <c r="AF30" s="11"/>
       <c r="AG30" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH30" s="84">
         <f t="shared" si="38"/>
@@ -7067,7 +7094,7 @@
       </c>
       <c r="AV30" s="11"/>
       <c r="AW30" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX30" s="84">
         <f t="shared" si="40"/>
@@ -7128,7 +7155,7 @@
     </row>
     <row r="31" spans="1:65" ht="14">
       <c r="A31" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="86">
         <v>289</v>
@@ -7173,7 +7200,7 @@
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R31" s="84">
         <f t="shared" si="25"/>
@@ -7229,7 +7256,7 @@
         <v>4467</v>
       </c>
       <c r="AG31" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AH31" s="84">
         <f t="shared" si="38"/>
@@ -7285,7 +7312,7 @@
         <v>8067</v>
       </c>
       <c r="AW31" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX31" s="84">
         <f t="shared" si="40"/>
@@ -7581,7 +7608,7 @@
     </row>
     <row r="33" spans="1:63" ht="14">
       <c r="A33" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="49">
         <f>AVERAGE(B20:B29)</f>
@@ -7641,7 +7668,7 @@
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R33" s="49">
         <f>AVERAGE(R20:R29)</f>
@@ -7700,7 +7727,7 @@
         <v>4233</v>
       </c>
       <c r="AG33" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH33" s="49">
         <f>AVERAGE(AH20:AH29)</f>
@@ -7759,7 +7786,7 @@
         <v>7833</v>
       </c>
       <c r="AW33" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AX33" s="49">
         <f>AVERAGE(AX20:AX29)</f>
@@ -8204,7 +8231,7 @@
         <v>15</v>
       </c>
       <c r="O37" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q37" s="81" t="s">
         <v>2</v>
@@ -8249,7 +8276,7 @@
         <v>15</v>
       </c>
       <c r="AE37" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG37" s="31" t="s">
         <v>2</v>
@@ -8294,7 +8321,7 @@
         <v>15</v>
       </c>
       <c r="AU37" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AW37" s="31" t="s">
         <v>2</v>
@@ -8339,12 +8366,12 @@
         <v>15</v>
       </c>
       <c r="BK37" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:63" ht="14">
       <c r="A38" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="86">
         <f>B7+300</f>
@@ -8400,7 +8427,7 @@
       </c>
       <c r="O38" s="97"/>
       <c r="Q38" s="71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R38" s="84">
         <f>B38+1200</f>
@@ -8455,7 +8482,7 @@
       </c>
       <c r="AE38" s="97"/>
       <c r="AG38" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AH38" s="84">
         <f>R38+1200</f>
@@ -8510,7 +8537,7 @@
       </c>
       <c r="AU38" s="97"/>
       <c r="AW38" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AX38" s="84">
         <f>AH38+1200</f>
@@ -8567,7 +8594,7 @@
     </row>
     <row r="39" spans="1:63" ht="14">
       <c r="A39" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="86">
         <f t="shared" ref="B39:M39" si="95">B8+300</f>
@@ -8626,7 +8653,7 @@
         <v>939</v>
       </c>
       <c r="Q39" s="72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R39" s="84">
         <f t="shared" ref="R39:R62" si="98">B39+1200</f>
@@ -8684,7 +8711,7 @@
         <v>4539</v>
       </c>
       <c r="AG39" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH39" s="84">
         <f t="shared" ref="AH39:AH62" si="100">R39+1200</f>
@@ -8742,7 +8769,7 @@
         <v>8139</v>
       </c>
       <c r="AW39" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX39" s="84">
         <f t="shared" ref="AX39:AX62" si="102">AH39+1200</f>
@@ -8802,7 +8829,7 @@
     </row>
     <row r="40" spans="1:63" ht="14">
       <c r="A40" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="86">
         <f t="shared" ref="B40:M40" si="104">B9+300</f>
@@ -8861,7 +8888,7 @@
         <v>975</v>
       </c>
       <c r="Q40" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R40" s="84">
         <f t="shared" si="98"/>
@@ -8919,7 +8946,7 @@
         <v>4575</v>
       </c>
       <c r="AG40" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH40" s="84">
         <f t="shared" si="100"/>
@@ -8977,7 +9004,7 @@
         <v>8175</v>
       </c>
       <c r="AW40" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX40" s="84">
         <f t="shared" si="102"/>
@@ -9037,7 +9064,7 @@
     </row>
     <row r="41" spans="1:63" ht="14">
       <c r="A41" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="86">
         <f t="shared" ref="B41:M41" si="105">B10+300</f>
@@ -9096,7 +9123,7 @@
         <v>1011</v>
       </c>
       <c r="Q41" s="72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R41" s="84">
         <f t="shared" si="98"/>
@@ -9154,7 +9181,7 @@
         <v>4611</v>
       </c>
       <c r="AG41" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH41" s="84">
         <f t="shared" si="100"/>
@@ -9212,7 +9239,7 @@
         <v>8211</v>
       </c>
       <c r="AW41" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX41" s="84">
         <f t="shared" si="102"/>
@@ -9272,7 +9299,7 @@
     </row>
     <row r="42" spans="1:63" ht="14">
       <c r="A42" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="86">
         <f t="shared" ref="B42:M42" si="106">B11+300</f>
@@ -9331,7 +9358,7 @@
         <v>1047</v>
       </c>
       <c r="Q42" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R42" s="84">
         <f t="shared" si="98"/>
@@ -9389,7 +9416,7 @@
         <v>4647</v>
       </c>
       <c r="AG42" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH42" s="84">
         <f t="shared" si="100"/>
@@ -9447,7 +9474,7 @@
         <v>8247</v>
       </c>
       <c r="AW42" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX42" s="84">
         <f t="shared" si="102"/>
@@ -9507,7 +9534,7 @@
     </row>
     <row r="43" spans="1:63" ht="14">
       <c r="A43" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="86">
         <f t="shared" ref="B43:M43" si="107">B12+300</f>
@@ -9566,7 +9593,7 @@
         <v>1083</v>
       </c>
       <c r="Q43" s="72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R43" s="84">
         <f t="shared" si="98"/>
@@ -9624,7 +9651,7 @@
         <v>4683</v>
       </c>
       <c r="AG43" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH43" s="84">
         <f t="shared" si="100"/>
@@ -9682,7 +9709,7 @@
         <v>8283</v>
       </c>
       <c r="AW43" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AX43" s="84">
         <f t="shared" si="102"/>
@@ -9742,7 +9769,7 @@
     </row>
     <row r="44" spans="1:63" ht="14">
       <c r="A44" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B44" s="86">
         <f t="shared" ref="B44:M44" si="108">B13+300</f>
@@ -9801,7 +9828,7 @@
         <v>1119</v>
       </c>
       <c r="Q44" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R44" s="84">
         <f t="shared" si="98"/>
@@ -9859,7 +9886,7 @@
         <v>4719</v>
       </c>
       <c r="AG44" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AH44" s="84">
         <f t="shared" si="100"/>
@@ -9918,7 +9945,7 @@
         <v>8319</v>
       </c>
       <c r="AW44" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AX44" s="84">
         <f t="shared" si="102"/>
@@ -9979,7 +10006,7 @@
     </row>
     <row r="45" spans="1:63" ht="14">
       <c r="A45" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="86">
         <f t="shared" ref="B45:M45" si="109">B14+300</f>
@@ -10038,7 +10065,7 @@
         <v>1155</v>
       </c>
       <c r="Q45" s="72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R45" s="84">
         <f t="shared" si="98"/>
@@ -10097,7 +10124,7 @@
         <v>4755</v>
       </c>
       <c r="AG45" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH45" s="84">
         <f t="shared" si="100"/>
@@ -10156,7 +10183,7 @@
         <v>8355</v>
       </c>
       <c r="AW45" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX45" s="84">
         <f t="shared" si="102"/>
@@ -10217,7 +10244,7 @@
     </row>
     <row r="46" spans="1:63" ht="14">
       <c r="A46" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="86">
         <f t="shared" ref="B46:M46" si="110">B15+300</f>
@@ -10276,7 +10303,7 @@
         <v>1191</v>
       </c>
       <c r="Q46" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R46" s="84">
         <f t="shared" si="98"/>
@@ -10335,7 +10362,7 @@
         <v>4791</v>
       </c>
       <c r="AG46" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH46" s="84">
         <f t="shared" si="100"/>
@@ -10394,7 +10421,7 @@
         <v>8391</v>
       </c>
       <c r="AW46" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX46" s="84">
         <f t="shared" si="102"/>
@@ -10455,7 +10482,7 @@
     </row>
     <row r="47" spans="1:63" ht="14">
       <c r="A47" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="86">
         <f t="shared" ref="B47:M47" si="111">B16+300</f>
@@ -10514,7 +10541,7 @@
         <v>1227</v>
       </c>
       <c r="Q47" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R47" s="84">
         <f t="shared" si="98"/>
@@ -10573,7 +10600,7 @@
         <v>4827</v>
       </c>
       <c r="AG47" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH47" s="84">
         <f t="shared" si="100"/>
@@ -10632,7 +10659,7 @@
         <v>8427</v>
       </c>
       <c r="AW47" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AX47" s="84">
         <f t="shared" si="102"/>
@@ -10693,7 +10720,7 @@
     </row>
     <row r="48" spans="1:63" ht="14">
       <c r="A48" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="86">
         <f t="shared" ref="B48:M48" si="112">B17+300</f>
@@ -10752,7 +10779,7 @@
         <v>1263</v>
       </c>
       <c r="Q48" s="71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R48" s="84">
         <f t="shared" si="98"/>
@@ -10810,7 +10837,7 @@
         <v>4863</v>
       </c>
       <c r="AG48" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH48" s="84">
         <f t="shared" si="100"/>
@@ -10868,7 +10895,7 @@
         <v>8463</v>
       </c>
       <c r="AW48" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX48" s="84">
         <f t="shared" si="102"/>
@@ -10928,7 +10955,7 @@
     </row>
     <row r="49" spans="1:63" ht="14">
       <c r="A49" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="86">
         <f t="shared" ref="B49:M49" si="113">B18+300</f>
@@ -10987,7 +11014,7 @@
         <v>1299</v>
       </c>
       <c r="Q49" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R49" s="84">
         <f t="shared" si="98"/>
@@ -11046,7 +11073,7 @@
         <v>4899</v>
       </c>
       <c r="AG49" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH49" s="84">
         <f t="shared" si="100"/>
@@ -11105,7 +11132,7 @@
         <v>8499</v>
       </c>
       <c r="AW49" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX49" s="84">
         <f t="shared" si="102"/>
@@ -11166,7 +11193,7 @@
     </row>
     <row r="50" spans="1:63" ht="14">
       <c r="A50" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="86">
         <f t="shared" ref="B50:M50" si="114">B19+300</f>
@@ -11225,7 +11252,7 @@
         <v>1335</v>
       </c>
       <c r="Q50" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R50" s="84">
         <f t="shared" si="98"/>
@@ -11283,7 +11310,7 @@
         <v>4935</v>
       </c>
       <c r="AG50" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH50" s="84">
         <f t="shared" si="100"/>
@@ -11341,7 +11368,7 @@
         <v>8535</v>
       </c>
       <c r="AW50" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX50" s="84">
         <f t="shared" si="102"/>
@@ -11401,7 +11428,7 @@
     </row>
     <row r="51" spans="1:63" ht="14">
       <c r="A51" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="86">
         <f t="shared" ref="B51:M51" si="115">B20+300</f>
@@ -11460,7 +11487,7 @@
         <v>1371</v>
       </c>
       <c r="Q51" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R51" s="84">
         <f t="shared" si="98"/>
@@ -11519,7 +11546,7 @@
         <v>4971</v>
       </c>
       <c r="AG51" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH51" s="84">
         <f t="shared" si="100"/>
@@ -11578,7 +11605,7 @@
         <v>8571</v>
       </c>
       <c r="AW51" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX51" s="84">
         <f t="shared" si="102"/>
@@ -11639,7 +11666,7 @@
     </row>
     <row r="52" spans="1:63" ht="14">
       <c r="A52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="86">
         <f t="shared" ref="B52:M52" si="119">B21+300</f>
@@ -11698,7 +11725,7 @@
         <v>1407</v>
       </c>
       <c r="Q52" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R52" s="84">
         <f t="shared" si="98"/>
@@ -11757,7 +11784,7 @@
         <v>5007</v>
       </c>
       <c r="AG52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH52" s="84">
         <f t="shared" si="100"/>
@@ -11816,7 +11843,7 @@
         <v>8607</v>
       </c>
       <c r="AW52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX52" s="84">
         <f t="shared" si="102"/>
@@ -11877,7 +11904,7 @@
     </row>
     <row r="53" spans="1:63" ht="14">
       <c r="A53" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="86">
         <f t="shared" ref="B53:M53" si="120">B22+300</f>
@@ -11937,7 +11964,7 @@
       </c>
       <c r="P53" s="11"/>
       <c r="Q53" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R53" s="84">
         <f t="shared" si="98"/>
@@ -11997,7 +12024,7 @@
       </c>
       <c r="AF53" s="11"/>
       <c r="AG53" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH53" s="84">
         <f t="shared" si="100"/>
@@ -12057,7 +12084,7 @@
       </c>
       <c r="AV53" s="11"/>
       <c r="AW53" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX53" s="84">
         <f t="shared" si="102"/>
@@ -12118,7 +12145,7 @@
     </row>
     <row r="54" spans="1:63" ht="14">
       <c r="A54" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" s="86">
         <f t="shared" ref="B54:M54" si="121">B23+300</f>
@@ -12177,7 +12204,7 @@
         <v>1479</v>
       </c>
       <c r="Q54" s="71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R54" s="84">
         <f t="shared" si="98"/>
@@ -12236,7 +12263,7 @@
         <v>5079</v>
       </c>
       <c r="AG54" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH54" s="84">
         <f t="shared" si="100"/>
@@ -12295,7 +12322,7 @@
         <v>8679</v>
       </c>
       <c r="AW54" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX54" s="84">
         <f t="shared" si="102"/>
@@ -12356,7 +12383,7 @@
     </row>
     <row r="55" spans="1:63" ht="14">
       <c r="A55" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B55" s="86">
         <f t="shared" ref="B55:M55" si="123">B24+300</f>
@@ -12415,7 +12442,7 @@
         <v>1515</v>
       </c>
       <c r="Q55" s="72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R55" s="84">
         <f t="shared" si="98"/>
@@ -12474,7 +12501,7 @@
         <v>5115</v>
       </c>
       <c r="AG55" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH55" s="84">
         <f t="shared" si="100"/>
@@ -12533,7 +12560,7 @@
         <v>8715</v>
       </c>
       <c r="AW55" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX55" s="84">
         <f t="shared" si="102"/>
@@ -12594,7 +12621,7 @@
     </row>
     <row r="56" spans="1:63" ht="14">
       <c r="A56" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B56" s="86">
         <f t="shared" ref="B56:M56" si="124">B25+300</f>
@@ -12653,7 +12680,7 @@
         <v>1551</v>
       </c>
       <c r="Q56" s="71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R56" s="84">
         <f t="shared" si="98"/>
@@ -12712,7 +12739,7 @@
         <v>5151</v>
       </c>
       <c r="AG56" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH56" s="84">
         <f t="shared" si="100"/>
@@ -12771,7 +12798,7 @@
         <v>8751</v>
       </c>
       <c r="AW56" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AX56" s="84">
         <f t="shared" si="102"/>
@@ -12832,7 +12859,7 @@
     </row>
     <row r="57" spans="1:63" ht="14">
       <c r="A57" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="86">
         <f t="shared" ref="B57:M57" si="125">B26+300</f>
@@ -12891,7 +12918,7 @@
         <v>1587</v>
       </c>
       <c r="Q57" s="72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R57" s="84">
         <f t="shared" si="98"/>
@@ -12950,7 +12977,7 @@
         <v>5187</v>
       </c>
       <c r="AG57" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH57" s="84">
         <f t="shared" si="100"/>
@@ -13009,7 +13036,7 @@
         <v>8787</v>
       </c>
       <c r="AW57" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX57" s="84">
         <f t="shared" si="102"/>
@@ -13070,7 +13097,7 @@
     </row>
     <row r="58" spans="1:63" ht="14">
       <c r="A58" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" s="86">
         <f t="shared" ref="B58:M58" si="126">B27+300</f>
@@ -13129,7 +13156,7 @@
         <v>1623</v>
       </c>
       <c r="Q58" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R58" s="84">
         <f t="shared" si="98"/>
@@ -13188,7 +13215,7 @@
         <v>5223</v>
       </c>
       <c r="AG58" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH58" s="84">
         <f t="shared" si="100"/>
@@ -13247,7 +13274,7 @@
         <v>8823</v>
       </c>
       <c r="AW58" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX58" s="84">
         <f t="shared" si="102"/>
@@ -13308,7 +13335,7 @@
     </row>
     <row r="59" spans="1:63" ht="14">
       <c r="A59" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="86">
         <f t="shared" ref="B59:M59" si="127">B28+300</f>
@@ -13367,7 +13394,7 @@
         <v>1659</v>
       </c>
       <c r="Q59" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R59" s="84">
         <f t="shared" si="98"/>
@@ -13426,7 +13453,7 @@
         <v>5259</v>
       </c>
       <c r="AG59" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH59" s="84">
         <f t="shared" si="100"/>
@@ -13485,7 +13512,7 @@
         <v>8859</v>
       </c>
       <c r="AW59" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AX59" s="84">
         <f t="shared" si="102"/>
@@ -13546,7 +13573,7 @@
     </row>
     <row r="60" spans="1:63" ht="14">
       <c r="A60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="86">
         <f t="shared" ref="B60:M60" si="128">B29+300</f>
@@ -13605,7 +13632,7 @@
         <v>1695</v>
       </c>
       <c r="Q60" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R60" s="84">
         <f t="shared" si="98"/>
@@ -13664,7 +13691,7 @@
         <v>5295</v>
       </c>
       <c r="AG60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH60" s="84">
         <f t="shared" si="100"/>
@@ -13723,7 +13750,7 @@
         <v>8895</v>
       </c>
       <c r="AW60" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX60" s="84">
         <f t="shared" si="102"/>
@@ -13784,7 +13811,7 @@
     </row>
     <row r="61" spans="1:63" ht="14">
       <c r="A61" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61" s="86">
         <f t="shared" ref="B61:M61" si="129">B30+300</f>
@@ -13843,7 +13870,7 @@
         <v>1731</v>
       </c>
       <c r="Q61" s="72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R61" s="84">
         <f t="shared" si="98"/>
@@ -13902,7 +13929,7 @@
         <v>5331</v>
       </c>
       <c r="AG61" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH61" s="84">
         <f t="shared" si="100"/>
@@ -13961,7 +13988,7 @@
         <v>8931</v>
       </c>
       <c r="AW61" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX61" s="84">
         <f t="shared" si="102"/>
@@ -14022,7 +14049,7 @@
     </row>
     <row r="62" spans="1:63" ht="14">
       <c r="A62" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62" s="86">
         <f t="shared" ref="B62:M62" si="130">B31+300</f>
@@ -14078,7 +14105,7 @@
         <v>1767</v>
       </c>
       <c r="Q62" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R62" s="84">
         <f t="shared" si="98"/>
@@ -14134,7 +14161,7 @@
         <v>5367</v>
       </c>
       <c r="AG62" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AH62" s="84">
         <f t="shared" si="100"/>
@@ -14190,7 +14217,7 @@
         <v>8967</v>
       </c>
       <c r="AW62" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX62" s="84">
         <f t="shared" si="102"/>
@@ -14480,7 +14507,7 @@
     </row>
     <row r="64" spans="1:63" ht="14">
       <c r="A64" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" s="49">
         <f>AVERAGE(B51:B60)</f>
@@ -14539,7 +14566,7 @@
         <v>1533</v>
       </c>
       <c r="Q64" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R64" s="49">
         <f>AVERAGE(R51:R60)</f>
@@ -14598,7 +14625,7 @@
         <v>5133</v>
       </c>
       <c r="AG64" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH64" s="49">
         <f>AVERAGE(AH51:AH60)</f>
@@ -14657,7 +14684,7 @@
         <v>8733</v>
       </c>
       <c r="AW64" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AX64" s="49">
         <f>AVERAGE(AX51:AX60)</f>
@@ -15120,7 +15147,7 @@
         <v>15</v>
       </c>
       <c r="O68" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q68" s="81" t="s">
         <v>2</v>
@@ -15165,7 +15192,7 @@
         <v>15</v>
       </c>
       <c r="AE68" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG68" s="31" t="s">
         <v>2</v>
@@ -15210,7 +15237,7 @@
         <v>15</v>
       </c>
       <c r="AU68" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AW68" s="31" t="s">
         <v>2</v>
@@ -15255,12 +15282,12 @@
         <v>15</v>
       </c>
       <c r="BK68" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:63" ht="14">
       <c r="A69" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B69" s="86">
         <f>B38+300</f>
@@ -15316,7 +15343,7 @@
       </c>
       <c r="O69" s="97"/>
       <c r="Q69" s="71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R69" s="84">
         <f>B69+1200</f>
@@ -15367,12 +15394,12 @@
         <v>1812</v>
       </c>
       <c r="AD69" s="64">
-        <f t="shared" ref="R69:AD69" si="161">+AD100-(AD38+AD7)</f>
+        <f t="shared" ref="AD69" si="161">+AD100-(AD38+AD7)</f>
         <v>705.77750000000015</v>
       </c>
       <c r="AE69" s="97"/>
       <c r="AG69" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AH69" s="84">
         <f>R69+1200</f>
@@ -15427,7 +15454,7 @@
       </c>
       <c r="AU69" s="97"/>
       <c r="AW69" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AX69" s="84">
         <f>AH69+1200</f>
@@ -15484,7 +15511,7 @@
     </row>
     <row r="70" spans="1:63" ht="14">
       <c r="A70" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="86">
         <f t="shared" ref="B70:M70" si="184">B39+300</f>
@@ -15543,7 +15570,7 @@
         <v>1839</v>
       </c>
       <c r="Q70" s="72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R70" s="84">
         <f t="shared" ref="R70:R93" si="187">B70+1200</f>
@@ -15594,7 +15621,7 @@
         <v>1824</v>
       </c>
       <c r="AD70" s="64">
-        <f t="shared" ref="R70:AD70" si="188">+AD101-(AD39+AD8)</f>
+        <f t="shared" ref="AD70" si="188">+AD101-(AD39+AD8)</f>
         <v>2554.082399999992</v>
       </c>
       <c r="AE70" s="112">
@@ -15602,7 +15629,7 @@
         <v>5439</v>
       </c>
       <c r="AG70" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH70" s="84">
         <f t="shared" ref="AH70:AH93" si="190">R70+1200</f>
@@ -15660,7 +15687,7 @@
         <v>9039</v>
       </c>
       <c r="AW70" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX70" s="84">
         <f t="shared" ref="AX70:AX93" si="192">AH70+1200</f>
@@ -15720,7 +15747,7 @@
     </row>
     <row r="71" spans="1:63" ht="14">
       <c r="A71" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71" s="86">
         <f t="shared" ref="B71:M71" si="194">B40+300</f>
@@ -15779,7 +15806,7 @@
         <v>1875</v>
       </c>
       <c r="Q71" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R71" s="84">
         <f t="shared" si="187"/>
@@ -15830,7 +15857,7 @@
         <v>1836</v>
       </c>
       <c r="AD71" s="64">
-        <f t="shared" ref="R71:AD71" si="195">+AD102-(AD40+AD9)</f>
+        <f t="shared" ref="AD71" si="195">+AD102-(AD40+AD9)</f>
         <v>4680.6575000000012</v>
       </c>
       <c r="AE71" s="112">
@@ -15838,7 +15865,7 @@
         <v>5475</v>
       </c>
       <c r="AG71" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH71" s="84">
         <f t="shared" si="190"/>
@@ -15896,7 +15923,7 @@
         <v>9075</v>
       </c>
       <c r="AW71" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX71" s="84">
         <f t="shared" si="192"/>
@@ -15956,7 +15983,7 @@
     </row>
     <row r="72" spans="1:63" ht="14">
       <c r="A72" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B72" s="86">
         <f t="shared" ref="B72:M72" si="196">B41+300</f>
@@ -16015,7 +16042,7 @@
         <v>1911</v>
       </c>
       <c r="Q72" s="72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R72" s="84">
         <f t="shared" si="187"/>
@@ -16066,7 +16093,7 @@
         <v>1848</v>
       </c>
       <c r="AD72" s="64">
-        <f t="shared" ref="R72:AD72" si="197">+AD103-(AD41+AD10)</f>
+        <f t="shared" ref="AD72" si="197">+AD103-(AD41+AD10)</f>
         <v>656.09259999999995</v>
       </c>
       <c r="AE72" s="112">
@@ -16074,7 +16101,7 @@
         <v>5511</v>
       </c>
       <c r="AG72" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH72" s="84">
         <f t="shared" si="190"/>
@@ -16132,7 +16159,7 @@
         <v>9111</v>
       </c>
       <c r="AW72" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX72" s="84">
         <f t="shared" si="192"/>
@@ -16192,7 +16219,7 @@
     </row>
     <row r="73" spans="1:63" ht="14">
       <c r="A73" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B73" s="86">
         <f t="shared" ref="B73:M73" si="198">B42+300</f>
@@ -16251,7 +16278,7 @@
         <v>1947</v>
       </c>
       <c r="Q73" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R73" s="84">
         <f t="shared" si="187"/>
@@ -16302,7 +16329,7 @@
         <v>1860</v>
       </c>
       <c r="AD73" s="64">
-        <f t="shared" ref="R73:AD73" si="199">+AD104-(AD42+AD11)</f>
+        <f t="shared" ref="AD73" si="199">+AD104-(AD42+AD11)</f>
         <v>936.40170000000035</v>
       </c>
       <c r="AE73" s="112">
@@ -16310,7 +16337,7 @@
         <v>5547</v>
       </c>
       <c r="AG73" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH73" s="84">
         <f t="shared" si="190"/>
@@ -16368,7 +16395,7 @@
         <v>9147</v>
       </c>
       <c r="AW73" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX73" s="84">
         <f t="shared" si="192"/>
@@ -16428,7 +16455,7 @@
     </row>
     <row r="74" spans="1:63" ht="14">
       <c r="A74" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" s="86">
         <f t="shared" ref="B74:M74" si="200">B43+300</f>
@@ -16487,7 +16514,7 @@
         <v>1983</v>
       </c>
       <c r="Q74" s="72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R74" s="84">
         <f t="shared" si="187"/>
@@ -16538,7 +16565,7 @@
         <v>1872</v>
       </c>
       <c r="AD74" s="64">
-        <f t="shared" ref="R74:AD74" si="201">+AD105-(AD43+AD12)</f>
+        <f t="shared" ref="AD74" si="201">+AD105-(AD43+AD12)</f>
         <v>575.81239999999525</v>
       </c>
       <c r="AE74" s="112">
@@ -16546,7 +16573,7 @@
         <v>5583</v>
       </c>
       <c r="AG74" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH74" s="84">
         <f t="shared" si="190"/>
@@ -16604,7 +16631,7 @@
         <v>9183</v>
       </c>
       <c r="AW74" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AX74" s="84">
         <f t="shared" si="192"/>
@@ -16664,7 +16691,7 @@
     </row>
     <row r="75" spans="1:63" ht="14">
       <c r="A75" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B75" s="86">
         <f t="shared" ref="B75:M75" si="202">B44+300</f>
@@ -16723,7 +16750,7 @@
         <v>2019</v>
       </c>
       <c r="Q75" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R75" s="84">
         <f t="shared" si="187"/>
@@ -16774,7 +16801,7 @@
         <v>1884</v>
       </c>
       <c r="AD75" s="64">
-        <f t="shared" ref="R75:AD75" si="203">+AD106-(AD44+AD13)</f>
+        <f t="shared" ref="AD75" si="203">+AD106-(AD44+AD13)</f>
         <v>1060.6156999999985</v>
       </c>
       <c r="AE75" s="112">
@@ -16782,7 +16809,7 @@
         <v>5619</v>
       </c>
       <c r="AG75" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AH75" s="84">
         <f t="shared" si="190"/>
@@ -16841,7 +16868,7 @@
         <v>9219</v>
       </c>
       <c r="AW75" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AX75" s="84">
         <f t="shared" si="192"/>
@@ -16902,7 +16929,7 @@
     </row>
     <row r="76" spans="1:63" ht="14">
       <c r="A76" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B76" s="86">
         <f t="shared" ref="B76:M76" si="204">B45+300</f>
@@ -16961,7 +16988,7 @@
         <v>2055</v>
       </c>
       <c r="Q76" s="72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R76" s="84">
         <f t="shared" si="187"/>
@@ -17020,7 +17047,7 @@
         <v>5655</v>
       </c>
       <c r="AG76" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH76" s="84">
         <f t="shared" si="190"/>
@@ -17079,7 +17106,7 @@
         <v>9255</v>
       </c>
       <c r="AW76" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX76" s="84">
         <f t="shared" si="192"/>
@@ -17140,7 +17167,7 @@
     </row>
     <row r="77" spans="1:63" ht="14">
       <c r="A77" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77" s="86">
         <f t="shared" ref="B77:M77" si="205">B46+300</f>
@@ -17199,7 +17226,7 @@
         <v>2091</v>
       </c>
       <c r="Q77" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R77" s="84">
         <f t="shared" si="187"/>
@@ -17258,7 +17285,7 @@
         <v>5691</v>
       </c>
       <c r="AG77" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH77" s="84">
         <f t="shared" si="190"/>
@@ -17317,7 +17344,7 @@
         <v>9291</v>
       </c>
       <c r="AW77" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX77" s="84">
         <f t="shared" si="192"/>
@@ -17378,7 +17405,7 @@
     </row>
     <row r="78" spans="1:63" ht="14">
       <c r="A78" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" s="86">
         <f t="shared" ref="B78:M78" si="206">B47+300</f>
@@ -17437,7 +17464,7 @@
         <v>2127</v>
       </c>
       <c r="Q78" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R78" s="84">
         <f t="shared" si="187"/>
@@ -17496,7 +17523,7 @@
         <v>5727</v>
       </c>
       <c r="AG78" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH78" s="84">
         <f t="shared" si="190"/>
@@ -17555,7 +17582,7 @@
         <v>9327</v>
       </c>
       <c r="AW78" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AX78" s="84">
         <f t="shared" si="192"/>
@@ -17616,7 +17643,7 @@
     </row>
     <row r="79" spans="1:63" ht="14">
       <c r="A79" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" s="86">
         <f t="shared" ref="B79:M79" si="207">B48+300</f>
@@ -17675,7 +17702,7 @@
         <v>2163</v>
       </c>
       <c r="Q79" s="71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R79" s="84">
         <f t="shared" si="187"/>
@@ -17733,7 +17760,7 @@
         <v>5763</v>
       </c>
       <c r="AG79" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH79" s="84">
         <f t="shared" si="190"/>
@@ -17791,7 +17818,7 @@
         <v>9363</v>
       </c>
       <c r="AW79" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX79" s="84">
         <f t="shared" si="192"/>
@@ -17851,7 +17878,7 @@
     </row>
     <row r="80" spans="1:63" ht="14">
       <c r="A80" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B80" s="86">
         <f t="shared" ref="B80:M80" si="208">B49+300</f>
@@ -17910,7 +17937,7 @@
         <v>2199</v>
       </c>
       <c r="Q80" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R80" s="84">
         <f t="shared" si="187"/>
@@ -17969,7 +17996,7 @@
         <v>5799</v>
       </c>
       <c r="AG80" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH80" s="84">
         <f t="shared" si="190"/>
@@ -18028,7 +18055,7 @@
         <v>9399</v>
       </c>
       <c r="AW80" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX80" s="84">
         <f t="shared" si="192"/>
@@ -18089,7 +18116,7 @@
     </row>
     <row r="81" spans="1:65" ht="14">
       <c r="A81" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B81" s="86">
         <f t="shared" ref="B81:M81" si="209">B50+300</f>
@@ -18148,7 +18175,7 @@
         <v>2235</v>
       </c>
       <c r="Q81" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R81" s="84">
         <f t="shared" si="187"/>
@@ -18206,7 +18233,7 @@
         <v>5835</v>
       </c>
       <c r="AG81" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH81" s="84">
         <f t="shared" si="190"/>
@@ -18264,7 +18291,7 @@
         <v>9435</v>
       </c>
       <c r="AW81" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX81" s="84">
         <f t="shared" si="192"/>
@@ -18324,7 +18351,7 @@
     </row>
     <row r="82" spans="1:65" ht="14">
       <c r="A82" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="86">
         <f t="shared" ref="B82:M82" si="210">B51+300</f>
@@ -18383,7 +18410,7 @@
         <v>2271</v>
       </c>
       <c r="Q82" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R82" s="84">
         <f t="shared" si="187"/>
@@ -18442,7 +18469,7 @@
         <v>5871</v>
       </c>
       <c r="AG82" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH82" s="84">
         <f t="shared" si="190"/>
@@ -18501,7 +18528,7 @@
         <v>9471</v>
       </c>
       <c r="AW82" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX82" s="84">
         <f t="shared" si="192"/>
@@ -18562,7 +18589,7 @@
     </row>
     <row r="83" spans="1:65" ht="14">
       <c r="A83" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="86">
         <f t="shared" ref="B83:M83" si="214">B52+300</f>
@@ -18621,7 +18648,7 @@
         <v>2307</v>
       </c>
       <c r="Q83" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R83" s="84">
         <f t="shared" si="187"/>
@@ -18680,7 +18707,7 @@
         <v>5907</v>
       </c>
       <c r="AG83" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH83" s="84">
         <f t="shared" si="190"/>
@@ -18739,7 +18766,7 @@
         <v>9507</v>
       </c>
       <c r="AW83" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX83" s="84">
         <f t="shared" si="192"/>
@@ -18800,7 +18827,7 @@
     </row>
     <row r="84" spans="1:65" ht="14">
       <c r="A84" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84" s="86">
         <f t="shared" ref="B84:M84" si="215">B53+300</f>
@@ -18860,7 +18887,7 @@
       </c>
       <c r="P84" s="11"/>
       <c r="Q84" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R84" s="84">
         <f t="shared" si="187"/>
@@ -18920,7 +18947,7 @@
       </c>
       <c r="AF84" s="11"/>
       <c r="AG84" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH84" s="84">
         <f t="shared" si="190"/>
@@ -18980,7 +19007,7 @@
       </c>
       <c r="AV84" s="11"/>
       <c r="AW84" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX84" s="84">
         <f t="shared" si="192"/>
@@ -19042,7 +19069,7 @@
     </row>
     <row r="85" spans="1:65" ht="14">
       <c r="A85" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B85" s="86">
         <f t="shared" ref="B85:M85" si="216">B54+300</f>
@@ -19101,7 +19128,7 @@
         <v>2379</v>
       </c>
       <c r="Q85" s="71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R85" s="84">
         <f t="shared" si="187"/>
@@ -19160,7 +19187,7 @@
         <v>5979</v>
       </c>
       <c r="AG85" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH85" s="84">
         <f t="shared" si="190"/>
@@ -19219,7 +19246,7 @@
         <v>9579</v>
       </c>
       <c r="AW85" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX85" s="84">
         <f t="shared" si="192"/>
@@ -19280,7 +19307,7 @@
     </row>
     <row r="86" spans="1:65" ht="14">
       <c r="A86" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86" s="86">
         <f t="shared" ref="B86:M86" si="218">B55+300</f>
@@ -19339,7 +19366,7 @@
         <v>2415</v>
       </c>
       <c r="Q86" s="72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R86" s="84">
         <f t="shared" si="187"/>
@@ -19398,7 +19425,7 @@
         <v>6015</v>
       </c>
       <c r="AG86" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH86" s="84">
         <f t="shared" si="190"/>
@@ -19457,7 +19484,7 @@
         <v>9615</v>
       </c>
       <c r="AW86" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX86" s="84">
         <f t="shared" si="192"/>
@@ -19518,7 +19545,7 @@
     </row>
     <row r="87" spans="1:65" ht="14">
       <c r="A87" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="86">
         <f t="shared" ref="B87:M87" si="219">B56+300</f>
@@ -19577,7 +19604,7 @@
         <v>2451</v>
       </c>
       <c r="Q87" s="71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R87" s="84">
         <f t="shared" si="187"/>
@@ -19636,7 +19663,7 @@
         <v>6051</v>
       </c>
       <c r="AG87" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH87" s="84">
         <f t="shared" si="190"/>
@@ -19695,7 +19722,7 @@
         <v>9651</v>
       </c>
       <c r="AW87" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AX87" s="84">
         <f t="shared" si="192"/>
@@ -19756,7 +19783,7 @@
     </row>
     <row r="88" spans="1:65" ht="14">
       <c r="A88" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B88" s="86">
         <f t="shared" ref="B88:M88" si="220">B57+300</f>
@@ -19815,7 +19842,7 @@
         <v>2487</v>
       </c>
       <c r="Q88" s="72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R88" s="84">
         <f t="shared" si="187"/>
@@ -19874,7 +19901,7 @@
         <v>6087</v>
       </c>
       <c r="AG88" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH88" s="84">
         <f t="shared" si="190"/>
@@ -19933,7 +19960,7 @@
         <v>9687</v>
       </c>
       <c r="AW88" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX88" s="84">
         <f t="shared" si="192"/>
@@ -19994,7 +20021,7 @@
     </row>
     <row r="89" spans="1:65" ht="14">
       <c r="A89" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B89" s="86">
         <f t="shared" ref="B89:M89" si="221">B58+300</f>
@@ -20053,7 +20080,7 @@
         <v>2523</v>
       </c>
       <c r="Q89" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R89" s="84">
         <f t="shared" si="187"/>
@@ -20112,7 +20139,7 @@
         <v>6123</v>
       </c>
       <c r="AG89" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH89" s="84">
         <f t="shared" si="190"/>
@@ -20171,7 +20198,7 @@
         <v>9723</v>
       </c>
       <c r="AW89" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX89" s="84">
         <f t="shared" si="192"/>
@@ -20233,7 +20260,7 @@
     </row>
     <row r="90" spans="1:65" ht="14">
       <c r="A90" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B90" s="86">
         <f t="shared" ref="B90:M90" si="222">B59+300</f>
@@ -20292,7 +20319,7 @@
         <v>2559</v>
       </c>
       <c r="Q90" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R90" s="84">
         <f t="shared" si="187"/>
@@ -20351,7 +20378,7 @@
         <v>6159</v>
       </c>
       <c r="AG90" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH90" s="84">
         <f t="shared" si="190"/>
@@ -20410,7 +20437,7 @@
         <v>9759</v>
       </c>
       <c r="AW90" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AX90" s="84">
         <f t="shared" si="192"/>
@@ -20472,7 +20499,7 @@
     </row>
     <row r="91" spans="1:65" ht="14">
       <c r="A91" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="86">
         <f t="shared" ref="B91:M91" si="223">B60+300</f>
@@ -20531,7 +20558,7 @@
         <v>2595</v>
       </c>
       <c r="Q91" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R91" s="84">
         <f t="shared" si="187"/>
@@ -20590,7 +20617,7 @@
         <v>6195</v>
       </c>
       <c r="AG91" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH91" s="84">
         <f t="shared" si="190"/>
@@ -20649,7 +20676,7 @@
         <v>9795</v>
       </c>
       <c r="AW91" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX91" s="84">
         <f t="shared" si="192"/>
@@ -20711,7 +20738,7 @@
     </row>
     <row r="92" spans="1:65" ht="14">
       <c r="A92" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B92" s="86">
         <f t="shared" ref="B92:M92" si="224">B61+300</f>
@@ -20770,7 +20797,7 @@
         <v>2631</v>
       </c>
       <c r="Q92" s="72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R92" s="84">
         <f t="shared" si="187"/>
@@ -20829,7 +20856,7 @@
         <v>6231</v>
       </c>
       <c r="AG92" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH92" s="84">
         <f t="shared" si="190"/>
@@ -20888,7 +20915,7 @@
         <v>9831</v>
       </c>
       <c r="AW92" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX92" s="84">
         <f t="shared" si="192"/>
@@ -20950,7 +20977,7 @@
     </row>
     <row r="93" spans="1:65" ht="14">
       <c r="A93" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B93" s="86">
         <f t="shared" ref="B93:M93" si="225">B62+300</f>
@@ -21006,7 +21033,7 @@
         <v>2667</v>
       </c>
       <c r="Q93" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R93" s="84">
         <f t="shared" si="187"/>
@@ -21062,7 +21089,7 @@
         <v>6267</v>
       </c>
       <c r="AG93" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AH93" s="84">
         <f t="shared" si="190"/>
@@ -21118,7 +21145,7 @@
         <v>9867</v>
       </c>
       <c r="AW93" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX93" s="84">
         <f t="shared" si="192"/>
@@ -21409,7 +21436,7 @@
     </row>
     <row r="95" spans="1:65" ht="14">
       <c r="A95" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B95" s="49">
         <f>AVERAGE(B82:B91)</f>
@@ -21468,7 +21495,7 @@
         <v>2433</v>
       </c>
       <c r="Q95" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R95" s="49">
         <f>AVERAGE(R82:R91)</f>
@@ -21527,7 +21554,7 @@
         <v>6033</v>
       </c>
       <c r="AG95" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH95" s="49">
         <f>AVERAGE(AH82:AH91)</f>
@@ -21586,7 +21613,7 @@
         <v>9633</v>
       </c>
       <c r="AW95" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AX95" s="49">
         <f>AVERAGE(AX82:AX91)</f>
@@ -22049,7 +22076,7 @@
         <v>15</v>
       </c>
       <c r="O99" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q99" s="81" t="s">
         <v>2</v>
@@ -22094,7 +22121,7 @@
         <v>15</v>
       </c>
       <c r="AE99" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG99" s="31" t="s">
         <v>2</v>
@@ -22139,7 +22166,7 @@
         <v>15</v>
       </c>
       <c r="AU99" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AW99" s="31" t="s">
         <v>2</v>
@@ -22184,12 +22211,12 @@
         <v>15</v>
       </c>
       <c r="BK99" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:63" ht="14">
       <c r="A100" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B100" s="86">
         <f>B69+300</f>
@@ -22245,7 +22272,7 @@
       </c>
       <c r="O100" s="97"/>
       <c r="Q100" s="71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R100" s="84">
         <f>B100+1200</f>
@@ -22300,7 +22327,7 @@
       </c>
       <c r="AE100" s="97"/>
       <c r="AG100" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AH100" s="84">
         <f>R100+1200</f>
@@ -22355,7 +22382,7 @@
       </c>
       <c r="AU100" s="97"/>
       <c r="AW100" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AX100" s="84">
         <f>AH100+1200</f>
@@ -22412,7 +22439,7 @@
     </row>
     <row r="101" spans="1:63" ht="14">
       <c r="A101" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B101" s="86">
         <f t="shared" ref="B101:M101" si="276">B70+300</f>
@@ -22471,7 +22498,7 @@
         <v>2739</v>
       </c>
       <c r="Q101" s="72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R101" s="84">
         <f t="shared" ref="R101:R124" si="279">B101+1200</f>
@@ -22529,7 +22556,7 @@
         <v>6339</v>
       </c>
       <c r="AG101" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH101" s="84">
         <f t="shared" ref="AH101:AH124" si="281">R101+1200</f>
@@ -22587,7 +22614,7 @@
         <v>9939</v>
       </c>
       <c r="AW101" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX101" s="84">
         <f t="shared" ref="AX101:AX124" si="283">AH101+1200</f>
@@ -22647,7 +22674,7 @@
     </row>
     <row r="102" spans="1:63" ht="14">
       <c r="A102" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B102" s="86">
         <f t="shared" ref="B102:M102" si="285">B71+300</f>
@@ -22706,7 +22733,7 @@
         <v>2775</v>
       </c>
       <c r="Q102" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R102" s="84">
         <f t="shared" si="279"/>
@@ -22764,7 +22791,7 @@
         <v>6375</v>
       </c>
       <c r="AG102" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AH102" s="84">
         <f t="shared" si="281"/>
@@ -22822,7 +22849,7 @@
         <v>9975</v>
       </c>
       <c r="AW102" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX102" s="84">
         <f t="shared" si="283"/>
@@ -22882,7 +22909,7 @@
     </row>
     <row r="103" spans="1:63" ht="14">
       <c r="A103" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B103" s="86">
         <f t="shared" ref="B103:M103" si="286">B72+300</f>
@@ -22941,7 +22968,7 @@
         <v>2811</v>
       </c>
       <c r="Q103" s="72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R103" s="84">
         <f t="shared" si="279"/>
@@ -22999,7 +23026,7 @@
         <v>6411</v>
       </c>
       <c r="AG103" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH103" s="84">
         <f t="shared" si="281"/>
@@ -23057,7 +23084,7 @@
         <v>10011</v>
       </c>
       <c r="AW103" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX103" s="84">
         <f t="shared" si="283"/>
@@ -23117,7 +23144,7 @@
     </row>
     <row r="104" spans="1:63" ht="14">
       <c r="A104" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B104" s="86">
         <f t="shared" ref="B104:M104" si="287">B73+300</f>
@@ -23176,7 +23203,7 @@
         <v>2847</v>
       </c>
       <c r="Q104" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R104" s="84">
         <f t="shared" si="279"/>
@@ -23234,7 +23261,7 @@
         <v>6447</v>
       </c>
       <c r="AG104" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH104" s="84">
         <f t="shared" si="281"/>
@@ -23292,7 +23319,7 @@
         <v>10047</v>
       </c>
       <c r="AW104" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX104" s="84">
         <f t="shared" si="283"/>
@@ -23352,7 +23379,7 @@
     </row>
     <row r="105" spans="1:63" ht="14">
       <c r="A105" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B105" s="86">
         <f t="shared" ref="B105:M105" si="288">B74+300</f>
@@ -23411,7 +23438,7 @@
         <v>2883</v>
       </c>
       <c r="Q105" s="72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R105" s="84">
         <f t="shared" si="279"/>
@@ -23469,7 +23496,7 @@
         <v>6483</v>
       </c>
       <c r="AG105" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH105" s="84">
         <f t="shared" si="281"/>
@@ -23527,7 +23554,7 @@
         <v>10083</v>
       </c>
       <c r="AW105" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AX105" s="84">
         <f t="shared" si="283"/>
@@ -23587,7 +23614,7 @@
     </row>
     <row r="106" spans="1:63" ht="14">
       <c r="A106" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B106" s="86">
         <f t="shared" ref="B106:M106" si="289">B75+300</f>
@@ -23646,7 +23673,7 @@
         <v>2919</v>
       </c>
       <c r="Q106" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R106" s="84">
         <f t="shared" si="279"/>
@@ -23704,7 +23731,7 @@
         <v>6519</v>
       </c>
       <c r="AG106" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AH106" s="84">
         <f t="shared" si="281"/>
@@ -23763,7 +23790,7 @@
         <v>10119</v>
       </c>
       <c r="AW106" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AX106" s="84">
         <f t="shared" si="283"/>
@@ -23824,7 +23851,7 @@
     </row>
     <row r="107" spans="1:63" ht="14">
       <c r="A107" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B107" s="86">
         <f t="shared" ref="B107:M107" si="290">B76+300</f>
@@ -23883,7 +23910,7 @@
         <v>2955</v>
       </c>
       <c r="Q107" s="72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R107" s="84">
         <f t="shared" si="279"/>
@@ -23942,7 +23969,7 @@
         <v>6555</v>
       </c>
       <c r="AG107" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH107" s="84">
         <f t="shared" si="281"/>
@@ -23993,7 +24020,7 @@
         <v>3396</v>
       </c>
       <c r="AT107" s="64">
-        <f t="shared" ref="AH107:AT107" si="291">+AT76+AT45+AT14</f>
+        <f t="shared" ref="AT107" si="291">+AT76+AT45+AT14</f>
         <v>100458</v>
       </c>
       <c r="AU107" s="112">
@@ -24001,7 +24028,7 @@
         <v>10155</v>
       </c>
       <c r="AW107" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX107" s="84">
         <f t="shared" si="283"/>
@@ -24062,7 +24089,7 @@
     </row>
     <row r="108" spans="1:63" ht="14">
       <c r="A108" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B108" s="86">
         <f t="shared" ref="B108:M108" si="292">B77+300</f>
@@ -24121,7 +24148,7 @@
         <v>2991</v>
       </c>
       <c r="Q108" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R108" s="84">
         <f t="shared" si="279"/>
@@ -24180,7 +24207,7 @@
         <v>6591</v>
       </c>
       <c r="AG108" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH108" s="84">
         <f t="shared" si="281"/>
@@ -24239,7 +24266,7 @@
         <v>10191</v>
       </c>
       <c r="AW108" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX108" s="84">
         <f t="shared" si="283"/>
@@ -24300,7 +24327,7 @@
     </row>
     <row r="109" spans="1:63" ht="14">
       <c r="A109" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B109" s="86">
         <f t="shared" ref="B109:M109" si="293">B78+300</f>
@@ -24359,7 +24386,7 @@
         <v>3027</v>
       </c>
       <c r="Q109" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R109" s="84">
         <f t="shared" si="279"/>
@@ -24418,7 +24445,7 @@
         <v>6627</v>
       </c>
       <c r="AG109" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH109" s="84">
         <f t="shared" si="281"/>
@@ -24477,7 +24504,7 @@
         <v>10227</v>
       </c>
       <c r="AW109" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AX109" s="84">
         <f t="shared" si="283"/>
@@ -24538,7 +24565,7 @@
     </row>
     <row r="110" spans="1:63" ht="14">
       <c r="A110" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B110" s="86">
         <f t="shared" ref="B110:M110" si="294">B79+300</f>
@@ -24597,7 +24624,7 @@
         <v>3063</v>
       </c>
       <c r="Q110" s="71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R110" s="84">
         <f t="shared" si="279"/>
@@ -24655,7 +24682,7 @@
         <v>6663</v>
       </c>
       <c r="AG110" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH110" s="84">
         <f t="shared" si="281"/>
@@ -24713,7 +24740,7 @@
         <v>10263</v>
       </c>
       <c r="AW110" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX110" s="84">
         <f t="shared" si="283"/>
@@ -24773,7 +24800,7 @@
     </row>
     <row r="111" spans="1:63" ht="14">
       <c r="A111" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B111" s="86">
         <f t="shared" ref="B111:M111" si="295">B80+300</f>
@@ -24832,7 +24859,7 @@
         <v>3099</v>
       </c>
       <c r="Q111" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R111" s="84">
         <f t="shared" si="279"/>
@@ -24891,7 +24918,7 @@
         <v>6699</v>
       </c>
       <c r="AG111" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH111" s="84">
         <f t="shared" si="281"/>
@@ -24950,7 +24977,7 @@
         <v>10299</v>
       </c>
       <c r="AW111" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX111" s="84">
         <f t="shared" si="283"/>
@@ -25011,7 +25038,7 @@
     </row>
     <row r="112" spans="1:63" ht="14">
       <c r="A112" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B112" s="86">
         <f t="shared" ref="B112:M112" si="296">B81+300</f>
@@ -25070,7 +25097,7 @@
         <v>3135</v>
       </c>
       <c r="Q112" s="71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R112" s="84">
         <f t="shared" si="279"/>
@@ -25128,7 +25155,7 @@
         <v>6735</v>
       </c>
       <c r="AG112" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AH112" s="84">
         <f t="shared" si="281"/>
@@ -25186,7 +25213,7 @@
         <v>10335</v>
       </c>
       <c r="AW112" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX112" s="84">
         <f t="shared" si="283"/>
@@ -25246,7 +25273,7 @@
     </row>
     <row r="113" spans="1:64" ht="14">
       <c r="A113" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B113" s="86">
         <f t="shared" ref="B113:M113" si="297">B82+300</f>
@@ -25305,7 +25332,7 @@
         <v>3171</v>
       </c>
       <c r="Q113" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R113" s="84">
         <f t="shared" si="279"/>
@@ -25364,7 +25391,7 @@
         <v>6771</v>
       </c>
       <c r="AG113" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH113" s="84">
         <f t="shared" si="281"/>
@@ -25423,7 +25450,7 @@
         <v>10371</v>
       </c>
       <c r="AW113" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX113" s="84">
         <f t="shared" si="283"/>
@@ -25484,7 +25511,7 @@
     </row>
     <row r="114" spans="1:64" ht="14">
       <c r="A114" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B114" s="86">
         <f t="shared" ref="B114:M114" si="299">B83+300</f>
@@ -25543,7 +25570,7 @@
         <v>3207</v>
       </c>
       <c r="Q114" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R114" s="84">
         <f t="shared" si="279"/>
@@ -25602,7 +25629,7 @@
         <v>6807</v>
       </c>
       <c r="AG114" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH114" s="84">
         <f t="shared" si="281"/>
@@ -25661,7 +25688,7 @@
         <v>10407</v>
       </c>
       <c r="AW114" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX114" s="84">
         <f t="shared" si="283"/>
@@ -25722,7 +25749,7 @@
     </row>
     <row r="115" spans="1:64" ht="14">
       <c r="A115" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B115" s="86">
         <f t="shared" ref="B115:M115" si="300">B84+300</f>
@@ -25782,7 +25809,7 @@
       </c>
       <c r="P115" s="11"/>
       <c r="Q115" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R115" s="84">
         <f t="shared" si="279"/>
@@ -25842,7 +25869,7 @@
       </c>
       <c r="AF115" s="11"/>
       <c r="AG115" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AH115" s="84">
         <f t="shared" si="281"/>
@@ -25901,7 +25928,7 @@
         <v>10443</v>
       </c>
       <c r="AW115" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX115" s="84">
         <f t="shared" si="283"/>
@@ -25962,7 +25989,7 @@
     </row>
     <row r="116" spans="1:64" ht="14">
       <c r="A116" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B116" s="86">
         <f t="shared" ref="B116:M116" si="301">B85+300</f>
@@ -26013,7 +26040,7 @@
         <v>1104</v>
       </c>
       <c r="N116" s="52">
-        <f t="shared" ref="B116:N116" si="302">N23+N54+N85</f>
+        <f t="shared" ref="N116" si="302">N23+N54+N85</f>
         <v>17946</v>
       </c>
       <c r="O116" s="112">
@@ -26021,7 +26048,7 @@
         <v>3279</v>
       </c>
       <c r="Q116" s="71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R116" s="84">
         <f t="shared" si="279"/>
@@ -26072,7 +26099,7 @@
         <v>2304</v>
       </c>
       <c r="AD116" s="64">
-        <f t="shared" ref="R116:AD116" si="303">AD23+AD54+AD85</f>
+        <f t="shared" ref="AD116" si="303">AD23+AD54+AD85</f>
         <v>61146</v>
       </c>
       <c r="AE116" s="112">
@@ -26080,7 +26107,7 @@
         <v>6879</v>
       </c>
       <c r="AG116" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH116" s="84">
         <f t="shared" si="281"/>
@@ -26139,7 +26166,7 @@
         <v>10479</v>
       </c>
       <c r="AW116" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX116" s="84">
         <f t="shared" si="283"/>
@@ -26190,7 +26217,7 @@
         <v>4704</v>
       </c>
       <c r="BJ116" s="52">
-        <f t="shared" ref="AX116:BJ116" si="304">BJ23+BJ54+BJ85</f>
+        <f t="shared" ref="BJ116" si="304">BJ23+BJ54+BJ85</f>
         <v>147546</v>
       </c>
       <c r="BK116" s="112">
@@ -26200,7 +26227,7 @@
     </row>
     <row r="117" spans="1:64" ht="14">
       <c r="A117" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B117" s="86">
         <f t="shared" ref="B117:M117" si="305">B86+300</f>
@@ -26251,7 +26278,7 @@
         <v>1116</v>
       </c>
       <c r="N117" s="52">
-        <f t="shared" ref="B117:N117" si="306">N24+N55+N86</f>
+        <f t="shared" ref="N117" si="306">N24+N55+N86</f>
         <v>18378</v>
       </c>
       <c r="O117" s="112">
@@ -26259,7 +26286,7 @@
         <v>3315</v>
       </c>
       <c r="Q117" s="72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R117" s="84">
         <f t="shared" si="279"/>
@@ -26310,7 +26337,7 @@
         <v>2316</v>
       </c>
       <c r="AD117" s="64">
-        <f t="shared" ref="R117:AD117" si="307">AD24+AD55+AD86</f>
+        <f t="shared" ref="AD117" si="307">AD24+AD55+AD86</f>
         <v>61578</v>
       </c>
       <c r="AE117" s="112">
@@ -26318,7 +26345,7 @@
         <v>6915</v>
       </c>
       <c r="AG117" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH117" s="84">
         <f t="shared" si="281"/>
@@ -26377,7 +26404,7 @@
         <v>10515</v>
       </c>
       <c r="AW117" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX117" s="84">
         <f t="shared" si="283"/>
@@ -26428,7 +26455,7 @@
         <v>4716</v>
       </c>
       <c r="BJ117" s="52">
-        <f t="shared" ref="AX117:BJ117" si="308">BJ24+BJ55+BJ86</f>
+        <f t="shared" ref="BJ117" si="308">BJ24+BJ55+BJ86</f>
         <v>147978</v>
       </c>
       <c r="BK117" s="112">
@@ -26438,7 +26465,7 @@
     </row>
     <row r="118" spans="1:64" ht="14">
       <c r="A118" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B118" s="86">
         <f t="shared" ref="B118:M118" si="309">B87+300</f>
@@ -26497,7 +26524,7 @@
         <v>3351</v>
       </c>
       <c r="Q118" s="71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R118" s="84">
         <f t="shared" si="279"/>
@@ -26556,7 +26583,7 @@
         <v>6951</v>
       </c>
       <c r="AG118" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH118" s="84">
         <f t="shared" si="281"/>
@@ -26615,7 +26642,7 @@
         <v>10551</v>
       </c>
       <c r="AW118" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AX118" s="84">
         <f t="shared" si="283"/>
@@ -26676,7 +26703,7 @@
     </row>
     <row r="119" spans="1:64" ht="14">
       <c r="A119" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B119" s="86">
         <f t="shared" ref="B119:M119" si="312">B88+300</f>
@@ -26735,7 +26762,7 @@
         <v>3387</v>
       </c>
       <c r="Q119" s="72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R119" s="84">
         <f t="shared" si="279"/>
@@ -26794,7 +26821,7 @@
         <v>6987</v>
       </c>
       <c r="AG119" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH119" s="84">
         <f t="shared" si="281"/>
@@ -26853,7 +26880,7 @@
         <v>10587</v>
       </c>
       <c r="AW119" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX119" s="84">
         <f t="shared" si="283"/>
@@ -26914,7 +26941,7 @@
     </row>
     <row r="120" spans="1:64" ht="14">
       <c r="A120" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B120" s="86">
         <f t="shared" ref="B120:M120" si="313">B89+300</f>
@@ -26973,7 +27000,7 @@
         <v>3423</v>
       </c>
       <c r="Q120" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R120" s="84">
         <f t="shared" si="279"/>
@@ -27032,7 +27059,7 @@
         <v>7023</v>
       </c>
       <c r="AG120" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH120" s="84">
         <f t="shared" si="281"/>
@@ -27091,7 +27118,7 @@
         <v>10623</v>
       </c>
       <c r="AW120" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX120" s="84">
         <f t="shared" si="283"/>
@@ -27152,7 +27179,7 @@
     </row>
     <row r="121" spans="1:64" ht="14">
       <c r="A121" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B121" s="86">
         <f t="shared" ref="B121:M121" si="314">B90+300</f>
@@ -27211,7 +27238,7 @@
         <v>3459</v>
       </c>
       <c r="Q121" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R121" s="84">
         <f t="shared" si="279"/>
@@ -27270,7 +27297,7 @@
         <v>7059</v>
       </c>
       <c r="AG121" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH121" s="84">
         <f t="shared" si="281"/>
@@ -27329,7 +27356,7 @@
         <v>10659</v>
       </c>
       <c r="AW121" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AX121" s="84">
         <f t="shared" si="283"/>
@@ -27390,7 +27417,7 @@
     </row>
     <row r="122" spans="1:64" ht="14">
       <c r="A122" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B122" s="86">
         <f t="shared" ref="B122:M122" si="315">B91+300</f>
@@ -27449,7 +27476,7 @@
         <v>3495</v>
       </c>
       <c r="Q122" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R122" s="84">
         <f t="shared" si="279"/>
@@ -27500,7 +27527,7 @@
         <v>2376</v>
       </c>
       <c r="AD122" s="64">
-        <f t="shared" ref="T122:AD122" si="316">AD29+AD60+AD91</f>
+        <f t="shared" ref="AD122" si="316">AD29+AD60+AD91</f>
         <v>63738</v>
       </c>
       <c r="AE122" s="112">
@@ -27508,7 +27535,7 @@
         <v>7095</v>
       </c>
       <c r="AG122" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AH122" s="84">
         <f t="shared" si="281"/>
@@ -27567,7 +27594,7 @@
         <v>10695</v>
       </c>
       <c r="AW122" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX122" s="84">
         <f t="shared" si="283"/>
@@ -27628,7 +27655,7 @@
     </row>
     <row r="123" spans="1:64" ht="14">
       <c r="A123" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B123" s="86">
         <f t="shared" ref="B123:M123" si="317">B92+300</f>
@@ -27687,7 +27714,7 @@
         <v>3531</v>
       </c>
       <c r="Q123" s="72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R123" s="84">
         <f t="shared" si="279"/>
@@ -27746,7 +27773,7 @@
         <v>7131</v>
       </c>
       <c r="AG123" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH123" s="84">
         <f t="shared" si="281"/>
@@ -27805,7 +27832,7 @@
         <v>10731</v>
       </c>
       <c r="AW123" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX123" s="84">
         <f t="shared" si="283"/>
@@ -27866,7 +27893,7 @@
     </row>
     <row r="124" spans="1:64" ht="14">
       <c r="A124" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B124" s="86">
         <f t="shared" ref="B124:M124" si="318">B93+300</f>
@@ -27925,7 +27952,7 @@
         <v>3567</v>
       </c>
       <c r="Q124" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R124" s="84">
         <f t="shared" si="279"/>
@@ -27984,7 +28011,7 @@
         <v>7167</v>
       </c>
       <c r="AG124" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AH124" s="84">
         <f t="shared" si="281"/>
@@ -28035,7 +28062,7 @@
         <v>3600</v>
       </c>
       <c r="AT124" s="54">
-        <f t="shared" ref="AH123:AT124" si="320">AT31+AT62+AT93</f>
+        <f t="shared" ref="AT124" si="320">AT31+AT62+AT93</f>
         <v>0</v>
       </c>
       <c r="AU124" s="83">
@@ -28043,7 +28070,7 @@
         <v>10767</v>
       </c>
       <c r="AW124" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX124" s="84">
         <f t="shared" si="283"/>
@@ -28339,7 +28366,7 @@
     </row>
     <row r="126" spans="1:64" ht="14">
       <c r="A126" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B126" s="49">
         <f>AVERAGE(B113:B122)</f>
@@ -28398,7 +28425,7 @@
         <v>3333</v>
       </c>
       <c r="Q126" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R126" s="49">
         <f>AVERAGE(R113:R122)</f>
@@ -28457,7 +28484,7 @@
         <v>6933</v>
       </c>
       <c r="AG126" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH126" s="49">
         <f>AVERAGE(AH113:AH122)</f>
@@ -28516,7 +28543,7 @@
         <v>10533</v>
       </c>
       <c r="AW126" s="74" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AX126" s="49">
         <f>AVERAGE(AX113:AX122)</f>
@@ -28929,7 +28956,7 @@
       <c r="AS130" s="66"/>
       <c r="AT130" s="66"/>
       <c r="AW130" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX130" s="39"/>
       <c r="AY130" s="39"/>
@@ -29017,7 +29044,7 @@
         <v>15</v>
       </c>
       <c r="BK131" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="132" spans="1:63">
@@ -29046,7 +29073,7 @@
       <c r="AS132" s="66"/>
       <c r="AT132" s="66"/>
       <c r="AW132" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AX132" s="84">
         <v>4801</v>
@@ -29116,7 +29143,7 @@
       <c r="AS133" s="66"/>
       <c r="AT133" s="66"/>
       <c r="AW133" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX133" s="84">
         <v>4813</v>
@@ -29187,7 +29214,7 @@
       <c r="AS134" s="66"/>
       <c r="AT134" s="66"/>
       <c r="AW134" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX134" s="84">
         <v>4825</v>
@@ -29257,7 +29284,7 @@
       <c r="AS135" s="66"/>
       <c r="AT135" s="66"/>
       <c r="AW135" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX135" s="84">
         <v>4837</v>
@@ -29327,7 +29354,7 @@
       <c r="AS136" s="66"/>
       <c r="AT136" s="66"/>
       <c r="AW136" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AX136" s="84">
         <v>4849</v>
@@ -29398,7 +29425,7 @@
       <c r="AS137" s="66"/>
       <c r="AT137" s="66"/>
       <c r="AW137" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AX137" s="84">
         <v>4861</v>
@@ -29468,7 +29495,7 @@
       <c r="AS138" s="66"/>
       <c r="AT138" s="66"/>
       <c r="AW138" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AX138" s="84">
         <v>4873</v>
@@ -29538,7 +29565,7 @@
       <c r="AS139" s="66"/>
       <c r="AT139" s="66"/>
       <c r="AW139" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AX139" s="84">
         <v>4885</v>
@@ -29602,7 +29629,7 @@
       <c r="AS140" s="66"/>
       <c r="AT140" s="66"/>
       <c r="AW140" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX140" s="84">
         <v>4897</v>
@@ -29666,7 +29693,7 @@
       <c r="AS141" s="66"/>
       <c r="AT141" s="66"/>
       <c r="AW141" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AX141" s="84">
         <v>4909</v>
@@ -29730,7 +29757,7 @@
       <c r="AS142" s="66"/>
       <c r="AT142" s="66"/>
       <c r="AW142" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX142" s="84">
         <v>4921</v>
@@ -29794,7 +29821,7 @@
       <c r="AS143" s="66"/>
       <c r="AT143" s="66"/>
       <c r="AW143" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX143" s="84">
         <v>4933</v>
@@ -29852,7 +29879,7 @@
       <c r="AS144" s="66"/>
       <c r="AT144" s="66"/>
       <c r="AW144" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX144" s="84">
         <v>4945</v>
@@ -29910,7 +29937,7 @@
       <c r="AS145" s="66"/>
       <c r="AT145" s="66"/>
       <c r="AW145" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX145" s="84">
         <v>4957</v>
@@ -29968,7 +29995,7 @@
       <c r="AS146" s="66"/>
       <c r="AT146" s="66"/>
       <c r="AW146" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX146" s="84">
         <v>4969</v>
@@ -30026,7 +30053,7 @@
       <c r="AS147" s="66"/>
       <c r="AT147" s="66"/>
       <c r="AW147" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX147" s="84">
         <v>4981</v>
@@ -30084,7 +30111,7 @@
       <c r="AS148" s="66"/>
       <c r="AT148" s="66"/>
       <c r="AW148" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX148" s="84">
         <v>4993</v>
@@ -30142,7 +30169,7 @@
       <c r="AS149" s="66"/>
       <c r="AT149" s="66"/>
       <c r="AW149" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX149" s="84">
         <v>5005</v>
@@ -30188,7 +30215,7 @@
     </row>
     <row r="150" spans="35:63">
       <c r="AW150" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AX150" s="84">
         <v>5017</v>
@@ -30234,7 +30261,7 @@
     </row>
     <row r="151" spans="35:63">
       <c r="AW151" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX151" s="84">
         <v>5029</v>
@@ -30280,7 +30307,7 @@
     </row>
     <row r="152" spans="35:63">
       <c r="AW152" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AX152" s="84">
         <v>5041</v>
@@ -30326,7 +30353,7 @@
     </row>
     <row r="153" spans="35:63">
       <c r="AW153" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AX153" s="84">
         <v>5053</v>
@@ -30372,7 +30399,7 @@
     </row>
     <row r="154" spans="35:63">
       <c r="AW154" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AX154" s="84">
         <v>5065</v>
@@ -30418,7 +30445,7 @@
     </row>
     <row r="155" spans="35:63">
       <c r="AW155" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AX155" s="84">
         <v>5077</v>
@@ -30464,7 +30491,7 @@
     </row>
     <row r="156" spans="35:63">
       <c r="AW156" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX156" s="84">
         <v>5089</v>
@@ -30526,7 +30553,7 @@
     </row>
     <row r="158" spans="35:63">
       <c r="AW158" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX158" s="32"/>
       <c r="AY158" s="32"/>

</xml_diff>